<commit_message>
updated for July schedule
</commit_message>
<xml_diff>
--- a/シフトHTML変換.xlsx
+++ b/シフトHTML変換.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\host\br_website\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F00EE9-434D-43E5-A86A-6E28B7448E13}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="19395" windowHeight="2895"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,12 +18,19 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="98">
   <si>
     <t>1日月曜 柘榴</t>
   </si>
@@ -314,66 +327,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>1日木曜 柘榴</t>
-  </si>
-  <si>
-    <t>2日金曜 イリヤ</t>
-  </si>
-  <si>
-    <t>3日土曜 イリヤ</t>
-  </si>
-  <si>
-    <t>4日日曜 カーマ</t>
-  </si>
-  <si>
-    <t>5日月曜 休み</t>
-  </si>
-  <si>
-    <t>6日火曜 柘榴</t>
-  </si>
-  <si>
-    <t>7日水曜 カナ</t>
-  </si>
-  <si>
-    <t>8日木曜 イリヤ</t>
-  </si>
-  <si>
-    <t>9日金曜 美咲</t>
-  </si>
-  <si>
-    <t>10日土曜 美咲、カーマ</t>
-  </si>
-  <si>
-    <t>11日日曜 カナ</t>
-  </si>
-  <si>
-    <t>12日月曜 柘榴</t>
-  </si>
-  <si>
-    <t>13日火曜 カナ</t>
-  </si>
-  <si>
-    <t>14日水曜 柘榴</t>
-  </si>
-  <si>
-    <t>15日木曜 カーマ</t>
-  </si>
-  <si>
-    <t>16日金曜 イリヤ</t>
-  </si>
-  <si>
-    <t>17日土曜 美咲、イリヤ</t>
-  </si>
-  <si>
-    <t>18日日曜 柘榴</t>
-  </si>
-  <si>
-    <t>19日月曜 休み</t>
-  </si>
-  <si>
-    <t>20日火曜 柘榴</t>
-  </si>
-  <si>
     <t>21日水曜 カナ</t>
   </si>
   <si>
@@ -402,13 +355,55 @@
   </si>
   <si>
     <t>30日金曜 カーマ</t>
+  </si>
+  <si>
+    <t>1日月曜 カーマ</t>
+  </si>
+  <si>
+    <t>2日火曜 柘榴</t>
+  </si>
+  <si>
+    <t>3日水曜 カーマ</t>
+  </si>
+  <si>
+    <t>4日木曜 イリヤ</t>
+  </si>
+  <si>
+    <t>6日土曜 ことみ</t>
+  </si>
+  <si>
+    <t>7日日曜 柘榴</t>
+  </si>
+  <si>
+    <t>8日月曜 お休み</t>
+  </si>
+  <si>
+    <t>9日火曜 柘榴</t>
+  </si>
+  <si>
+    <t>10日水曜 カーマ</t>
+  </si>
+  <si>
+    <t>13日土曜 美咲、柘榴</t>
+  </si>
+  <si>
+    <t>14日日曜 カナ</t>
+  </si>
+  <si>
+    <t>15日月曜 カーマ</t>
+  </si>
+  <si>
+    <t>17日水曜 柘榴</t>
+  </si>
+  <si>
+    <t>20日土曜 美咲バースデー</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -530,6 +525,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -551,7 +549,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="角丸四角形 1"/>
+        <xdr:cNvPr id="2" name="角丸四角形 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -597,7 +601,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office ​​テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -639,7 +643,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -672,9 +676,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -707,6 +728,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -882,32 +920,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.25" style="2" customWidth="1"/>
-    <col min="3" max="3" width="7.125" style="2" customWidth="1"/>
-    <col min="4" max="5" width="10.625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="5.25" style="2" customWidth="1"/>
-    <col min="7" max="7" width="7.125" style="2" customWidth="1"/>
-    <col min="8" max="9" width="10.625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="5.25" style="2" customWidth="1"/>
-    <col min="11" max="11" width="7.125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="10.625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="4.125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="12.625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="112.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" style="2" customWidth="1"/>
+    <col min="4" max="5" width="10.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="5.21875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" style="2" customWidth="1"/>
+    <col min="8" max="9" width="10.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="5.21875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="7.109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="4.109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="112.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -954,9 +992,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B2" s="2">
         <v>2</v>
@@ -969,7 +1007,7 @@
       </c>
       <c r="E2" s="2" t="str">
         <f>REPLACE(A2,B2,C2,D2)</f>
-        <v>1日(木曜 柘榴</v>
+        <v>1日(月曜 カーマ</v>
       </c>
       <c r="F2" s="2">
         <v>5</v>
@@ -982,7 +1020,7 @@
       </c>
       <c r="I2" s="2" t="str">
         <f>REPLACE(E2,F2,G2,H2)</f>
-        <v>1日(木)&lt;/td&gt;&lt;td&gt; 柘榴</v>
+        <v>1日(月)&lt;/td&gt;&lt;td&gt; カーマ</v>
       </c>
       <c r="J2" s="2">
         <v>4</v>
@@ -995,20 +1033,20 @@
       </c>
       <c r="M2" s="2" t="str">
         <f>MID(I2,J2,K2)</f>
-        <v>木</v>
+        <v>月</v>
       </c>
       <c r="N2" s="2" t="str">
         <f t="shared" ref="N2:N11" si="0">IF(OR(M2="土", M2="日"), "&lt;tr class='weekend'&gt;&lt;td&gt;"&amp;I2, "&lt;tr&gt;&lt;td&gt;"&amp;I2)</f>
-        <v>&lt;tr&gt;&lt;td&gt;1日(木)&lt;/td&gt;&lt;td&gt; 柘榴</v>
+        <v>&lt;tr&gt;&lt;td&gt;1日(月)&lt;/td&gt;&lt;td&gt; カーマ</v>
       </c>
       <c r="O2" t="str">
         <f t="shared" ref="O2:O11" si="1">IF(M2="日", N2&amp;"&lt;span class='event_font'&gt;&amp;nbsp&amp;nbspセット料金半額DAY!&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;",N2&amp;"&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;1日(木)&lt;/td&gt;&lt;td&gt; 柘榴&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <v>&lt;tr&gt;&lt;td&gt;1日(月)&lt;/td&gt;&lt;td&gt; カーマ&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
@@ -1021,7 +1059,7 @@
       </c>
       <c r="E3" s="2" t="str">
         <f t="shared" ref="E3:E10" si="2">REPLACE(A3,B3,C3,D3)</f>
-        <v>2日(金曜 イリヤ</v>
+        <v>2日(火曜 柘榴</v>
       </c>
       <c r="F3" s="2">
         <v>5</v>
@@ -1034,7 +1072,7 @@
       </c>
       <c r="I3" s="2" t="str">
         <f t="shared" ref="I3:I10" si="3">REPLACE(E3,F3,G3,H3)</f>
-        <v>2日(金)&lt;/td&gt;&lt;td&gt; イリヤ</v>
+        <v>2日(火)&lt;/td&gt;&lt;td&gt; 柘榴</v>
       </c>
       <c r="J3" s="2">
         <v>4</v>
@@ -1047,20 +1085,20 @@
       </c>
       <c r="M3" s="2" t="str">
         <f t="shared" ref="M3:M32" si="4">MID(I3,J3,K3)</f>
-        <v>金</v>
+        <v>火</v>
       </c>
       <c r="N3" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;2日(金)&lt;/td&gt;&lt;td&gt; イリヤ</v>
+        <v>&lt;tr&gt;&lt;td&gt;2日(火)&lt;/td&gt;&lt;td&gt; 柘榴</v>
       </c>
       <c r="O3" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;2日(金)&lt;/td&gt;&lt;td&gt; イリヤ&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+        <v>&lt;tr&gt;&lt;td&gt;2日(火)&lt;/td&gt;&lt;td&gt; 柘榴&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
@@ -1073,7 +1111,7 @@
       </c>
       <c r="E4" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>3日(土曜 イリヤ</v>
+        <v>3日(水曜 カーマ</v>
       </c>
       <c r="F4" s="2">
         <v>5</v>
@@ -1086,7 +1124,7 @@
       </c>
       <c r="I4" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>3日(土)&lt;/td&gt;&lt;td&gt; イリヤ</v>
+        <v>3日(水)&lt;/td&gt;&lt;td&gt; カーマ</v>
       </c>
       <c r="J4" s="2">
         <v>4</v>
@@ -1099,20 +1137,20 @@
       </c>
       <c r="M4" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>土</v>
+        <v>水</v>
       </c>
       <c r="N4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr class='weekend'&gt;&lt;td&gt;3日(土)&lt;/td&gt;&lt;td&gt; イリヤ</v>
+        <v>&lt;tr&gt;&lt;td&gt;3日(水)&lt;/td&gt;&lt;td&gt; カーマ</v>
       </c>
       <c r="O4" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr class='weekend'&gt;&lt;td&gt;3日(土)&lt;/td&gt;&lt;td&gt; イリヤ&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+        <v>&lt;tr&gt;&lt;td&gt;3日(水)&lt;/td&gt;&lt;td&gt; カーマ&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
@@ -1125,7 +1163,7 @@
       </c>
       <c r="E5" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>4日(日曜 カーマ</v>
+        <v>4日(木曜 イリヤ</v>
       </c>
       <c r="F5" s="2">
         <v>5</v>
@@ -1138,7 +1176,7 @@
       </c>
       <c r="I5" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>4日(日)&lt;/td&gt;&lt;td&gt; カーマ</v>
+        <v>4日(木)&lt;/td&gt;&lt;td&gt; イリヤ</v>
       </c>
       <c r="J5" s="2">
         <v>4</v>
@@ -1151,20 +1189,20 @@
       </c>
       <c r="M5" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>日</v>
+        <v>木</v>
       </c>
       <c r="N5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr class='weekend'&gt;&lt;td&gt;4日(日)&lt;/td&gt;&lt;td&gt; カーマ</v>
+        <v>&lt;tr&gt;&lt;td&gt;4日(木)&lt;/td&gt;&lt;td&gt; イリヤ</v>
       </c>
       <c r="O5" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr class='weekend'&gt;&lt;td&gt;4日(日)&lt;/td&gt;&lt;td&gt; カーマ&lt;span class='event_font'&gt;&amp;nbsp&amp;nbspセット料金半額DAY!&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+        <v>&lt;tr&gt;&lt;td&gt;4日(木)&lt;/td&gt;&lt;td&gt; イリヤ&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>2</v>
@@ -1177,7 +1215,7 @@
       </c>
       <c r="E6" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>5日(月曜 休み</v>
+        <v>5日(金曜 美咲</v>
       </c>
       <c r="F6" s="2">
         <v>5</v>
@@ -1190,7 +1228,7 @@
       </c>
       <c r="I6" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>5日(月)&lt;/td&gt;&lt;td&gt; 休み</v>
+        <v>5日(金)&lt;/td&gt;&lt;td&gt; 美咲</v>
       </c>
       <c r="J6" s="2">
         <v>4</v>
@@ -1203,20 +1241,20 @@
       </c>
       <c r="M6" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>月</v>
+        <v>金</v>
       </c>
       <c r="N6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;5日(月)&lt;/td&gt;&lt;td&gt; 休み</v>
+        <v>&lt;tr&gt;&lt;td&gt;5日(金)&lt;/td&gt;&lt;td&gt; 美咲</v>
       </c>
       <c r="O6" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;5日(月)&lt;/td&gt;&lt;td&gt; 休み&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+        <v>&lt;tr&gt;&lt;td&gt;5日(金)&lt;/td&gt;&lt;td&gt; 美咲&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B7" s="2">
         <v>2</v>
@@ -1229,7 +1267,7 @@
       </c>
       <c r="E7" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>6日(火曜 柘榴</v>
+        <v>6日(土曜 ことみ</v>
       </c>
       <c r="F7" s="2">
         <v>5</v>
@@ -1242,7 +1280,7 @@
       </c>
       <c r="I7" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>6日(火)&lt;/td&gt;&lt;td&gt; 柘榴</v>
+        <v>6日(土)&lt;/td&gt;&lt;td&gt; ことみ</v>
       </c>
       <c r="J7" s="2">
         <v>4</v>
@@ -1255,20 +1293,20 @@
       </c>
       <c r="M7" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>火</v>
+        <v>土</v>
       </c>
       <c r="N7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;6日(火)&lt;/td&gt;&lt;td&gt; 柘榴</v>
+        <v>&lt;tr class='weekend'&gt;&lt;td&gt;6日(土)&lt;/td&gt;&lt;td&gt; ことみ</v>
       </c>
       <c r="O7" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;6日(火)&lt;/td&gt;&lt;td&gt; 柘榴&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+        <v>&lt;tr class='weekend'&gt;&lt;td&gt;6日(土)&lt;/td&gt;&lt;td&gt; ことみ&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B8" s="2">
         <v>2</v>
@@ -1281,7 +1319,7 @@
       </c>
       <c r="E8" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>7日(水曜 カナ</v>
+        <v>7日(日曜 柘榴</v>
       </c>
       <c r="F8" s="2">
         <v>5</v>
@@ -1294,7 +1332,7 @@
       </c>
       <c r="I8" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>7日(水)&lt;/td&gt;&lt;td&gt; カナ</v>
+        <v>7日(日)&lt;/td&gt;&lt;td&gt; 柘榴</v>
       </c>
       <c r="J8" s="2">
         <v>4</v>
@@ -1307,20 +1345,20 @@
       </c>
       <c r="M8" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>水</v>
+        <v>日</v>
       </c>
       <c r="N8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;7日(水)&lt;/td&gt;&lt;td&gt; カナ</v>
+        <v>&lt;tr class='weekend'&gt;&lt;td&gt;7日(日)&lt;/td&gt;&lt;td&gt; 柘榴</v>
       </c>
       <c r="O8" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;7日(水)&lt;/td&gt;&lt;td&gt; カナ&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+        <v>&lt;tr class='weekend'&gt;&lt;td&gt;7日(日)&lt;/td&gt;&lt;td&gt; 柘榴&lt;span class='event_font'&gt;&amp;nbsp&amp;nbspセット料金半額DAY!&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B9" s="2">
         <v>2</v>
@@ -1333,7 +1371,7 @@
       </c>
       <c r="E9" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>8日(木曜 イリヤ</v>
+        <v>8日(月曜 お休み</v>
       </c>
       <c r="F9" s="2">
         <v>5</v>
@@ -1346,7 +1384,7 @@
       </c>
       <c r="I9" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>8日(木)&lt;/td&gt;&lt;td&gt; イリヤ</v>
+        <v>8日(月)&lt;/td&gt;&lt;td&gt; お休み</v>
       </c>
       <c r="J9" s="2">
         <v>4</v>
@@ -1359,20 +1397,20 @@
       </c>
       <c r="M9" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>木</v>
+        <v>月</v>
       </c>
       <c r="N9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;8日(木)&lt;/td&gt;&lt;td&gt; イリヤ</v>
+        <v>&lt;tr&gt;&lt;td&gt;8日(月)&lt;/td&gt;&lt;td&gt; お休み</v>
       </c>
       <c r="O9" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;8日(木)&lt;/td&gt;&lt;td&gt; イリヤ&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+        <v>&lt;tr&gt;&lt;td&gt;8日(月)&lt;/td&gt;&lt;td&gt; お休み&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B10" s="2">
         <v>2</v>
@@ -1385,7 +1423,7 @@
       </c>
       <c r="E10" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>9日(金曜 美咲</v>
+        <v>9日(火曜 柘榴</v>
       </c>
       <c r="F10" s="2">
         <v>5</v>
@@ -1398,7 +1436,7 @@
       </c>
       <c r="I10" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>9日(金)&lt;/td&gt;&lt;td&gt; 美咲</v>
+        <v>9日(火)&lt;/td&gt;&lt;td&gt; 柘榴</v>
       </c>
       <c r="J10" s="2">
         <v>4</v>
@@ -1411,20 +1449,20 @@
       </c>
       <c r="M10" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>金</v>
+        <v>火</v>
       </c>
       <c r="N10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;9日(金)&lt;/td&gt;&lt;td&gt; 美咲</v>
+        <v>&lt;tr&gt;&lt;td&gt;9日(火)&lt;/td&gt;&lt;td&gt; 柘榴</v>
       </c>
       <c r="O10" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr&gt;&lt;td&gt;9日(金)&lt;/td&gt;&lt;td&gt; 美咲&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
+        <v>&lt;tr&gt;&lt;td&gt;9日(火)&lt;/td&gt;&lt;td&gt; 柘榴&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B11" s="2">
         <v>3</v>
@@ -1437,7 +1475,7 @@
       </c>
       <c r="E11" s="2" t="str">
         <f>REPLACE(A11,B11,C11,D11)</f>
-        <v>10日(土曜 美咲、カーマ</v>
+        <v>10日(水曜 カーマ</v>
       </c>
       <c r="F11" s="2">
         <v>6</v>
@@ -1450,7 +1488,7 @@
       </c>
       <c r="I11" s="2" t="str">
         <f>REPLACE(E11,F11,G11,H11)</f>
-        <v>10日(土)&lt;/td&gt;&lt;td&gt; 美咲、カーマ</v>
+        <v>10日(水)&lt;/td&gt;&lt;td&gt; カーマ</v>
       </c>
       <c r="J11" s="2">
         <v>5</v>
@@ -1463,20 +1501,20 @@
       </c>
       <c r="M11" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>土</v>
+        <v>水</v>
       </c>
       <c r="N11" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr class='weekend'&gt;&lt;td&gt;10日(土)&lt;/td&gt;&lt;td&gt; 美咲、カーマ</v>
+        <v>&lt;tr&gt;&lt;td&gt;10日(水)&lt;/td&gt;&lt;td&gt; カーマ</v>
       </c>
       <c r="O11" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;tr class='weekend'&gt;&lt;td&gt;10日(土)&lt;/td&gt;&lt;td&gt; 美咲、カーマ&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
+        <v>&lt;tr&gt;&lt;td&gt;10日(水)&lt;/td&gt;&lt;td&gt; カーマ&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>3</v>
@@ -1489,7 +1527,7 @@
       </c>
       <c r="E12" s="2" t="str">
         <f t="shared" ref="E12:E32" si="5">REPLACE(A12,B12,C12,D12)</f>
-        <v>11日(日曜 カナ</v>
+        <v>11日(木曜 イリヤ</v>
       </c>
       <c r="F12" s="2">
         <v>6</v>
@@ -1502,7 +1540,7 @@
       </c>
       <c r="I12" s="2" t="str">
         <f t="shared" ref="I12:I32" si="6">REPLACE(E12,F12,G12,H12)</f>
-        <v>11日(日)&lt;/td&gt;&lt;td&gt; カナ</v>
+        <v>11日(木)&lt;/td&gt;&lt;td&gt; イリヤ</v>
       </c>
       <c r="J12" s="2">
         <v>5</v>
@@ -1515,20 +1553,20 @@
       </c>
       <c r="M12" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>日</v>
+        <v>木</v>
       </c>
       <c r="N12" s="2" t="str">
         <f>IF(OR(M12="土", M12="日"), "&lt;tr class='weekend'&gt;&lt;td&gt;"&amp;I12, "&lt;tr&gt;&lt;td&gt;"&amp;I12)</f>
-        <v>&lt;tr class='weekend'&gt;&lt;td&gt;11日(日)&lt;/td&gt;&lt;td&gt; カナ</v>
+        <v>&lt;tr&gt;&lt;td&gt;11日(木)&lt;/td&gt;&lt;td&gt; イリヤ</v>
       </c>
       <c r="O12" t="str">
         <f>IF(M12="日", N12&amp;"&lt;span class='event_font'&gt;&amp;nbsp&amp;nbspセット料金半額DAY!&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;",N12&amp;"&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;tr class='weekend'&gt;&lt;td&gt;11日(日)&lt;/td&gt;&lt;td&gt; カナ&lt;span class='event_font'&gt;&amp;nbsp&amp;nbspセット料金半額DAY!&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
+        <v>&lt;tr&gt;&lt;td&gt;11日(木)&lt;/td&gt;&lt;td&gt; イリヤ&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>3</v>
@@ -1541,7 +1579,7 @@
       </c>
       <c r="E13" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>12日(月曜 柘榴</v>
+        <v>12日(金曜 美咲</v>
       </c>
       <c r="F13" s="2">
         <v>6</v>
@@ -1554,7 +1592,7 @@
       </c>
       <c r="I13" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>12日(月)&lt;/td&gt;&lt;td&gt; 柘榴</v>
+        <v>12日(金)&lt;/td&gt;&lt;td&gt; 美咲</v>
       </c>
       <c r="J13" s="2">
         <v>5</v>
@@ -1567,20 +1605,20 @@
       </c>
       <c r="M13" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>月</v>
+        <v>金</v>
       </c>
       <c r="N13" s="2" t="str">
         <f t="shared" ref="N13:N32" si="7">IF(OR(M13="土", M13="日"), "&lt;tr class='weekend'&gt;&lt;td&gt;"&amp;I13, "&lt;tr&gt;&lt;td&gt;"&amp;I13)</f>
-        <v>&lt;tr&gt;&lt;td&gt;12日(月)&lt;/td&gt;&lt;td&gt; 柘榴</v>
+        <v>&lt;tr&gt;&lt;td&gt;12日(金)&lt;/td&gt;&lt;td&gt; 美咲</v>
       </c>
       <c r="O13" t="str">
         <f t="shared" ref="O13:O32" si="8">IF(M13="日", N13&amp;"&lt;span class='event_font'&gt;&amp;nbsp&amp;nbspセット料金半額DAY!&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;",N13&amp;"&lt;/td&gt;&lt;/tr&gt;")</f>
-        <v>&lt;tr&gt;&lt;td&gt;12日(月)&lt;/td&gt;&lt;td&gt; 柘榴&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
+        <v>&lt;tr&gt;&lt;td&gt;12日(金)&lt;/td&gt;&lt;td&gt; 美咲&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B14" s="2">
         <v>3</v>
@@ -1593,7 +1631,7 @@
       </c>
       <c r="E14" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>13日(火曜 カナ</v>
+        <v>13日(土曜 美咲、柘榴</v>
       </c>
       <c r="F14" s="2">
         <v>6</v>
@@ -1606,7 +1644,7 @@
       </c>
       <c r="I14" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>13日(火)&lt;/td&gt;&lt;td&gt; カナ</v>
+        <v>13日(土)&lt;/td&gt;&lt;td&gt; 美咲、柘榴</v>
       </c>
       <c r="J14" s="2">
         <v>5</v>
@@ -1619,20 +1657,20 @@
       </c>
       <c r="M14" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>火</v>
+        <v>土</v>
       </c>
       <c r="N14" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>&lt;tr&gt;&lt;td&gt;13日(火)&lt;/td&gt;&lt;td&gt; カナ</v>
+        <v>&lt;tr class='weekend'&gt;&lt;td&gt;13日(土)&lt;/td&gt;&lt;td&gt; 美咲、柘榴</v>
       </c>
       <c r="O14" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;tr&gt;&lt;td&gt;13日(火)&lt;/td&gt;&lt;td&gt; カナ&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
+        <v>&lt;tr class='weekend'&gt;&lt;td&gt;13日(土)&lt;/td&gt;&lt;td&gt; 美咲、柘榴&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="B15" s="2">
         <v>3</v>
@@ -1645,7 +1683,7 @@
       </c>
       <c r="E15" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>14日(水曜 柘榴</v>
+        <v>14日(日曜 カナ</v>
       </c>
       <c r="F15" s="2">
         <v>6</v>
@@ -1658,7 +1696,7 @@
       </c>
       <c r="I15" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>14日(水)&lt;/td&gt;&lt;td&gt; 柘榴</v>
+        <v>14日(日)&lt;/td&gt;&lt;td&gt; カナ</v>
       </c>
       <c r="J15" s="2">
         <v>5</v>
@@ -1671,20 +1709,20 @@
       </c>
       <c r="M15" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>水</v>
+        <v>日</v>
       </c>
       <c r="N15" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>&lt;tr&gt;&lt;td&gt;14日(水)&lt;/td&gt;&lt;td&gt; 柘榴</v>
+        <v>&lt;tr class='weekend'&gt;&lt;td&gt;14日(日)&lt;/td&gt;&lt;td&gt; カナ</v>
       </c>
       <c r="O15" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;tr&gt;&lt;td&gt;14日(水)&lt;/td&gt;&lt;td&gt; 柘榴&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
+        <v>&lt;tr class='weekend'&gt;&lt;td&gt;14日(日)&lt;/td&gt;&lt;td&gt; カナ&lt;span class='event_font'&gt;&amp;nbsp&amp;nbspセット料金半額DAY!&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B16" s="2">
         <v>3</v>
@@ -1697,7 +1735,7 @@
       </c>
       <c r="E16" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>15日(木曜 カーマ</v>
+        <v>15日(月曜 カーマ</v>
       </c>
       <c r="F16" s="2">
         <v>6</v>
@@ -1710,7 +1748,7 @@
       </c>
       <c r="I16" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>15日(木)&lt;/td&gt;&lt;td&gt; カーマ</v>
+        <v>15日(月)&lt;/td&gt;&lt;td&gt; カーマ</v>
       </c>
       <c r="J16" s="2">
         <v>5</v>
@@ -1723,20 +1761,20 @@
       </c>
       <c r="M16" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>木</v>
+        <v>月</v>
       </c>
       <c r="N16" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>&lt;tr&gt;&lt;td&gt;15日(木)&lt;/td&gt;&lt;td&gt; カーマ</v>
+        <v>&lt;tr&gt;&lt;td&gt;15日(月)&lt;/td&gt;&lt;td&gt; カーマ</v>
       </c>
       <c r="O16" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;tr&gt;&lt;td&gt;15日(木)&lt;/td&gt;&lt;td&gt; カーマ&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
+        <v>&lt;tr&gt;&lt;td&gt;15日(月)&lt;/td&gt;&lt;td&gt; カーマ&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>3</v>
@@ -1749,7 +1787,7 @@
       </c>
       <c r="E17" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>16日(金曜 イリヤ</v>
+        <v>16日(火曜 柘榴</v>
       </c>
       <c r="F17" s="2">
         <v>6</v>
@@ -1762,7 +1800,7 @@
       </c>
       <c r="I17" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>16日(金)&lt;/td&gt;&lt;td&gt; イリヤ</v>
+        <v>16日(火)&lt;/td&gt;&lt;td&gt; 柘榴</v>
       </c>
       <c r="J17" s="2">
         <v>5</v>
@@ -1775,20 +1813,20 @@
       </c>
       <c r="M17" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>金</v>
+        <v>火</v>
       </c>
       <c r="N17" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>&lt;tr&gt;&lt;td&gt;16日(金)&lt;/td&gt;&lt;td&gt; イリヤ</v>
+        <v>&lt;tr&gt;&lt;td&gt;16日(火)&lt;/td&gt;&lt;td&gt; 柘榴</v>
       </c>
       <c r="O17" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;tr&gt;&lt;td&gt;16日(金)&lt;/td&gt;&lt;td&gt; イリヤ&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15">
+        <v>&lt;tr&gt;&lt;td&gt;16日(火)&lt;/td&gt;&lt;td&gt; 柘榴&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B18" s="2">
         <v>3</v>
@@ -1801,7 +1839,7 @@
       </c>
       <c r="E18" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>17日(土曜 美咲、イリヤ</v>
+        <v>17日(水曜 柘榴</v>
       </c>
       <c r="F18" s="2">
         <v>6</v>
@@ -1814,7 +1852,7 @@
       </c>
       <c r="I18" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>17日(土)&lt;/td&gt;&lt;td&gt; 美咲、イリヤ</v>
+        <v>17日(水)&lt;/td&gt;&lt;td&gt; 柘榴</v>
       </c>
       <c r="J18" s="2">
         <v>5</v>
@@ -1827,20 +1865,20 @@
       </c>
       <c r="M18" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>土</v>
+        <v>水</v>
       </c>
       <c r="N18" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>&lt;tr class='weekend'&gt;&lt;td&gt;17日(土)&lt;/td&gt;&lt;td&gt; 美咲、イリヤ</v>
+        <v>&lt;tr&gt;&lt;td&gt;17日(水)&lt;/td&gt;&lt;td&gt; 柘榴</v>
       </c>
       <c r="O18" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;tr class='weekend'&gt;&lt;td&gt;17日(土)&lt;/td&gt;&lt;td&gt; 美咲、イリヤ&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
+        <v>&lt;tr&gt;&lt;td&gt;17日(水)&lt;/td&gt;&lt;td&gt; 柘榴&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>3</v>
@@ -1853,7 +1891,7 @@
       </c>
       <c r="E19" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>18日(日曜 柘榴</v>
+        <v>18日(木曜 イリヤ</v>
       </c>
       <c r="F19" s="2">
         <v>6</v>
@@ -1866,7 +1904,7 @@
       </c>
       <c r="I19" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>18日(日)&lt;/td&gt;&lt;td&gt; 柘榴</v>
+        <v>18日(木)&lt;/td&gt;&lt;td&gt; イリヤ</v>
       </c>
       <c r="J19" s="2">
         <v>5</v>
@@ -1879,20 +1917,20 @@
       </c>
       <c r="M19" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>日</v>
+        <v>木</v>
       </c>
       <c r="N19" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>&lt;tr class='weekend'&gt;&lt;td&gt;18日(日)&lt;/td&gt;&lt;td&gt; 柘榴</v>
+        <v>&lt;tr&gt;&lt;td&gt;18日(木)&lt;/td&gt;&lt;td&gt; イリヤ</v>
       </c>
       <c r="O19" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;tr class='weekend'&gt;&lt;td&gt;18日(日)&lt;/td&gt;&lt;td&gt; 柘榴&lt;span class='event_font'&gt;&amp;nbsp&amp;nbspセット料金半額DAY!&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15">
+        <v>&lt;tr&gt;&lt;td&gt;18日(木)&lt;/td&gt;&lt;td&gt; イリヤ&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2">
         <v>3</v>
@@ -1905,7 +1943,7 @@
       </c>
       <c r="E20" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>19日(月曜 休み</v>
+        <v>19日(金曜 美咲</v>
       </c>
       <c r="F20" s="2">
         <v>6</v>
@@ -1918,7 +1956,7 @@
       </c>
       <c r="I20" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>19日(月)&lt;/td&gt;&lt;td&gt; 休み</v>
+        <v>19日(金)&lt;/td&gt;&lt;td&gt; 美咲</v>
       </c>
       <c r="J20" s="2">
         <v>5</v>
@@ -1931,20 +1969,20 @@
       </c>
       <c r="M20" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>月</v>
+        <v>金</v>
       </c>
       <c r="N20" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>&lt;tr&gt;&lt;td&gt;19日(月)&lt;/td&gt;&lt;td&gt; 休み</v>
+        <v>&lt;tr&gt;&lt;td&gt;19日(金)&lt;/td&gt;&lt;td&gt; 美咲</v>
       </c>
       <c r="O20" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;tr&gt;&lt;td&gt;19日(月)&lt;/td&gt;&lt;td&gt; 休み&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
+        <v>&lt;tr&gt;&lt;td&gt;19日(金)&lt;/td&gt;&lt;td&gt; 美咲&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B21" s="2">
         <v>3</v>
@@ -1957,7 +1995,7 @@
       </c>
       <c r="E21" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>20日(火曜 柘榴</v>
+        <v>20日(土曜 美咲バースデー</v>
       </c>
       <c r="F21" s="2">
         <v>6</v>
@@ -1970,7 +2008,7 @@
       </c>
       <c r="I21" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>20日(火)&lt;/td&gt;&lt;td&gt; 柘榴</v>
+        <v>20日(土)&lt;/td&gt;&lt;td&gt; 美咲バースデー</v>
       </c>
       <c r="J21" s="2">
         <v>5</v>
@@ -1983,20 +2021,20 @@
       </c>
       <c r="M21" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>火</v>
+        <v>土</v>
       </c>
       <c r="N21" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>&lt;tr&gt;&lt;td&gt;20日(火)&lt;/td&gt;&lt;td&gt; 柘榴</v>
+        <v>&lt;tr class='weekend'&gt;&lt;td&gt;20日(土)&lt;/td&gt;&lt;td&gt; 美咲バースデー</v>
       </c>
       <c r="O21" t="str">
         <f t="shared" si="8"/>
-        <v>&lt;tr&gt;&lt;td&gt;20日(火)&lt;/td&gt;&lt;td&gt; 柘榴&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15">
+        <v>&lt;tr class='weekend'&gt;&lt;td&gt;20日(土)&lt;/td&gt;&lt;td&gt; 美咲バースデー&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="B22" s="2">
         <v>3</v>
@@ -2046,9 +2084,9 @@
         <v>&lt;tr&gt;&lt;td&gt;21日(水)&lt;/td&gt;&lt;td&gt; カナ&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="B23" s="2">
         <v>3</v>
@@ -2098,9 +2136,9 @@
         <v>&lt;tr&gt;&lt;td&gt;22日(木)&lt;/td&gt;&lt;td&gt; カーマ&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="B24" s="2">
         <v>3</v>
@@ -2150,9 +2188,9 @@
         <v>&lt;tr&gt;&lt;td&gt;23日(金)&lt;/td&gt;&lt;td&gt; 美咲&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="B25" s="2">
         <v>3</v>
@@ -2202,9 +2240,9 @@
         <v>&lt;tr class='weekend'&gt;&lt;td&gt;24日(土)&lt;/td&gt;&lt;td&gt; 美咲&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="B26" s="2">
         <v>3</v>
@@ -2254,9 +2292,9 @@
         <v>&lt;tr class='weekend'&gt;&lt;td&gt;25日(日)&lt;/td&gt;&lt;td&gt; 柘榴&lt;span class='event_font'&gt;&amp;nbsp&amp;nbspセット料金半額DAY!&lt;/span&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="B27" s="2">
         <v>3</v>
@@ -2306,9 +2344,9 @@
         <v>&lt;tr&gt;&lt;td&gt;26日(月)&lt;/td&gt;&lt;td&gt; 柘榴&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="B28" s="2">
         <v>3</v>
@@ -2358,9 +2396,9 @@
         <v>&lt;tr&gt;&lt;td&gt;27日(火)&lt;/td&gt;&lt;td&gt; カナ&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="B29" s="2">
         <v>3</v>
@@ -2410,9 +2448,9 @@
         <v>&lt;tr&gt;&lt;td&gt;28日(水)&lt;/td&gt;&lt;td&gt; 柘榴&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="B30" s="2">
         <v>3</v>
@@ -2462,9 +2500,9 @@
         <v>&lt;tr&gt;&lt;td&gt;29日(木)&lt;/td&gt;&lt;td&gt; イリヤ&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="B31" s="2">
         <v>3</v>
@@ -2514,7 +2552,7 @@
         <v>&lt;tr&gt;&lt;td&gt;30日(金)&lt;/td&gt;&lt;td&gt; カーマ&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -2569,11 +2607,12 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:R32"/>
   <sheetViews>
@@ -2581,27 +2620,27 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="5.375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.25" style="2" customWidth="1"/>
-    <col min="5" max="5" width="7.125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="5.25" style="2" customWidth="1"/>
-    <col min="9" max="11" width="7.125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="8.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="10.625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="33.25" style="2" customWidth="1"/>
-    <col min="16" max="16" width="33.375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="67.25" style="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="67.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="5.21875" style="2" customWidth="1"/>
+    <col min="9" max="11" width="7.109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="8.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="33.21875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="33.33203125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="67.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="67.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="27" customHeight="1">
+    <row r="1" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -2636,7 +2675,7 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="5"/>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2701,7 +2740,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2766,7 +2805,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2831,7 +2870,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2896,7 +2935,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2961,7 +3000,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3026,7 +3065,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3091,7 +3130,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3156,7 +3195,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3221,7 +3260,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3286,7 +3325,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -3351,7 +3390,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -3416,7 +3455,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3481,7 +3520,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -3546,7 +3585,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -3611,7 +3650,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -3676,7 +3715,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -3741,7 +3780,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -3806,7 +3845,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -3871,7 +3910,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -3936,7 +3975,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -4001,7 +4040,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -4066,7 +4105,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -4131,7 +4170,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -4196,7 +4235,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -4261,7 +4300,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -4326,7 +4365,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -4391,7 +4430,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -4456,7 +4495,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -4521,7 +4560,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -4586,7 +4625,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -4659,13 +4698,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4673,13 +4712,13 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>